<commit_message>
change locators for release server
</commit_message>
<xml_diff>
--- a/ExcelFiles/PatientSummary.xlsx
+++ b/ExcelFiles/PatientSummary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riomed\Release_Server\Cellma4ClinicalAuto2\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E72909A-D848-400D-B320-4C0BA4569A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76F38F6-12BC-496A-A01E-F393E66C50C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="21" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="54" activeTab="59" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginDetails" sheetId="2" r:id="rId1"/>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1299" uniqueCount="656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1302" uniqueCount="659">
   <si>
     <t>username</t>
   </si>
@@ -1064,9 +1064,6 @@
     <t>cond_notes</t>
   </si>
   <si>
-    <t>Condition</t>
-  </si>
-  <si>
     <t>Erythematous condition</t>
   </si>
   <si>
@@ -1368,9 +1365,6 @@
   </si>
   <si>
     <t>For_User</t>
-  </si>
-  <si>
-    <t>Manoj Vyavahare, Consultant</t>
   </si>
   <si>
     <t>Added notes</t>
@@ -2074,6 +2068,21 @@
   </si>
   <si>
     <t>Rash</t>
+  </si>
+  <si>
+    <t>Conditions</t>
+  </si>
+  <si>
+    <t>Asthmatic bronchitis</t>
+  </si>
+  <si>
+    <t>25/05/2024</t>
+  </si>
+  <si>
+    <t>28/06/2024</t>
+  </si>
+  <si>
+    <t>Manoj Release, Doctor</t>
   </si>
 </sst>
 </file>
@@ -2474,26 +2483,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="B2" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>366</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>367</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="B4" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
     </row>
   </sheetData>
@@ -2591,7 +2600,7 @@
         <v>130</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="F2" t="s">
         <v>168</v>
@@ -2986,16 +2995,16 @@
         <v>159</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>157</v>
       </c>
       <c r="L2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="M2" t="s">
         <v>188</v>
@@ -3307,13 +3316,13 @@
     </row>
     <row r="2" spans="1:48" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" s="14" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>300</v>
@@ -3322,7 +3331,7 @@
         <v>50</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>51</v>
@@ -3442,7 +3451,7 @@
         <v>170</v>
       </c>
       <c r="B2" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="C2" t="s">
         <v>131</v>
@@ -3505,7 +3514,7 @@
         <v>170</v>
       </c>
       <c r="B2" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="C2" t="s">
         <v>117</v>
@@ -3556,7 +3565,7 @@
         <v>170</v>
       </c>
       <c r="B2" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="C2" t="s">
         <v>123</v>
@@ -3571,15 +3580,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C664057-036F-45F9-BB17-F131467544E4}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
@@ -3626,13 +3635,13 @@
       </c>
       <c r="D2" s="6" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>26/07/2025</v>
+        <v>03/08/2025</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>196</v>
       </c>
       <c r="F2" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>279</v>
@@ -3705,13 +3714,13 @@
       </c>
       <c r="D2" s="6" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>26/07/2025</v>
+        <v>03/08/2025</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>197</v>
       </c>
       <c r="F2" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>280</v>
@@ -3840,13 +3849,13 @@
         <v>210</v>
       </c>
       <c r="B2" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>103</v>
@@ -3947,11 +3956,11 @@
         <v>210</v>
       </c>
       <c r="B2" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="C2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45864</v>
+        <v>45872</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>103</v>
@@ -4017,7 +4026,7 @@
         <v>210</v>
       </c>
       <c r="B2" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="C2" t="s">
         <v>123</v>
@@ -4091,7 +4100,7 @@
         <v>229</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>136</v>
@@ -4217,7 +4226,7 @@
         <v>229</v>
       </c>
       <c r="B2" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>136</v>
@@ -4282,7 +4291,7 @@
     </row>
     <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="B2" t="s">
         <v>123</v>
@@ -4356,7 +4365,7 @@
         <v>243</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>136</v>
@@ -4454,7 +4463,7 @@
         <v>243</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>136</v>
@@ -4513,7 +4522,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="B2" t="s">
         <v>254</v>
@@ -4820,7 +4829,7 @@
         <v>69</v>
       </c>
       <c r="D1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E1" t="s">
         <v>70</v>
@@ -4915,13 +4924,13 @@
         <v>220</v>
       </c>
       <c r="B2" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>82</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="E2" t="s">
         <v>71</v>
@@ -4939,10 +4948,10 @@
         <v>103</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="L2" t="s">
         <v>176</v>
@@ -5087,7 +5096,7 @@
         <v>270</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>268</v>
@@ -5136,7 +5145,7 @@
         <v>270</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>271</v>
@@ -5181,7 +5190,7 @@
         <v>266</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C2" t="s">
         <v>272</v>
@@ -5226,7 +5235,7 @@
         <v>275</v>
       </c>
       <c r="B2" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>277</v>
@@ -5274,7 +5283,7 @@
         <v>275</v>
       </c>
       <c r="B2" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>276</v>
@@ -5319,7 +5328,7 @@
         <v>275</v>
       </c>
       <c r="B2" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="C2" t="s">
         <v>278</v>
@@ -5407,7 +5416,7 @@
         <v>282</v>
       </c>
       <c r="B2" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>204</v>
@@ -5548,7 +5557,7 @@
         <v>282</v>
       </c>
       <c r="B2" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>308</v>
@@ -5612,10 +5621,10 @@
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1194F774-EACE-44AC-9C8A-A1CC70FE36E1}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5649,22 +5658,27 @@
     </row>
     <row r="2" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>654</v>
+      </c>
+      <c r="B2" t="s">
+        <v>655</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>656</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>657</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="F2" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>319</v>
-      </c>
-      <c r="B2" t="s">
-        <v>320</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>321</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="F2" t="s">
-        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -5713,7 +5727,7 @@
         <v>69</v>
       </c>
       <c r="D1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E1" t="s">
         <v>70</v>
@@ -5785,7 +5799,7 @@
         <v>113</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="E2" t="s">
         <v>86</v>
@@ -5849,7 +5863,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5883,22 +5897,22 @@
     </row>
     <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>319</v>
+        <v>654</v>
       </c>
       <c r="B2" t="s">
+        <v>655</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>322</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -5908,10 +5922,10 @@
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06A0A6C0-CF2F-48B8-BAC5-F3E5690001A5}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5920,20 +5934,26 @@
     <col min="2" max="2" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>67</v>
       </c>
       <c r="B1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>319</v>
+        <v>654</v>
       </c>
       <c r="B2" t="s">
-        <v>320</v>
+        <v>655</v>
+      </c>
+      <c r="C2" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -5968,21 +5988,21 @@
         <v>126</v>
       </c>
       <c r="D1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>326</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>327</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" t="s">
         <v>328</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>329</v>
-      </c>
-      <c r="D2" t="s">
-        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -6018,21 +6038,21 @@
         <v>126</v>
       </c>
       <c r="D1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>326</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>327</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" t="s">
         <v>328</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>329</v>
-      </c>
-      <c r="D2" t="s">
-        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -6068,13 +6088,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>326</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>327</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>328</v>
-      </c>
       <c r="C2" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -6108,96 +6128,96 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B1" t="s">
         <v>332</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>333</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>334</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>335</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>336</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>337</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>338</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>339</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>340</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>341</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>342</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>343</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>344</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>345</v>
-      </c>
-      <c r="O1" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>346</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>347</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="C2" s="12" t="s">
         <v>348</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="12" t="s">
         <v>349</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="E2" s="12" t="s">
         <v>350</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="F2" t="s">
         <v>351</v>
       </c>
-      <c r="F2" t="s">
-        <v>352</v>
-      </c>
       <c r="G2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="H2" t="s">
         <v>98</v>
       </c>
       <c r="I2" t="s">
+        <v>352</v>
+      </c>
+      <c r="J2" t="s">
         <v>353</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>354</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>355</v>
-      </c>
-      <c r="L2" t="s">
-        <v>356</v>
       </c>
       <c r="M2" s="5" t="s">
         <v>316</v>
       </c>
       <c r="N2" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="O2" t="s">
         <v>357</v>
-      </c>
-      <c r="O2" t="s">
-        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -6228,72 +6248,72 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>358</v>
+      </c>
+      <c r="B1" t="s">
         <v>359</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>336</v>
+      </c>
+      <c r="D1" t="s">
+        <v>337</v>
+      </c>
+      <c r="E1" t="s">
+        <v>338</v>
+      </c>
+      <c r="F1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G1" t="s">
         <v>360</v>
-      </c>
-      <c r="C1" t="s">
-        <v>337</v>
-      </c>
-      <c r="D1" t="s">
-        <v>338</v>
-      </c>
-      <c r="E1" t="s">
-        <v>339</v>
-      </c>
-      <c r="F1" t="s">
-        <v>340</v>
-      </c>
-      <c r="G1" t="s">
-        <v>361</v>
       </c>
       <c r="H1" t="s">
         <v>298</v>
       </c>
       <c r="I1" t="s">
+        <v>343</v>
+      </c>
+      <c r="J1" t="s">
         <v>344</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>345</v>
-      </c>
-      <c r="K1" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>362</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>363</v>
-      </c>
       <c r="C2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E2" t="s">
         <v>98</v>
       </c>
       <c r="F2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>316</v>
       </c>
       <c r="J2" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="K2" t="s">
         <v>357</v>
-      </c>
-      <c r="K2" t="s">
-        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -6334,93 +6354,93 @@
         <v>68</v>
       </c>
       <c r="C1" t="s">
+        <v>370</v>
+      </c>
+      <c r="D1" t="s">
         <v>371</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>372</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>373</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>374</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>375</v>
       </c>
-      <c r="H1" t="s">
-        <v>376</v>
-      </c>
       <c r="I1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="J1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="K1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="L1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="M1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="N1" t="s">
+        <v>392</v>
+      </c>
+      <c r="O1" t="s">
         <v>393</v>
-      </c>
-      <c r="O1" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B2" t="s">
+        <v>369</v>
+      </c>
+      <c r="C2" t="s">
+        <v>376</v>
+      </c>
+      <c r="D2" t="s">
+        <v>377</v>
+      </c>
+      <c r="E2" t="s">
+        <v>378</v>
+      </c>
+      <c r="F2" t="s">
+        <v>379</v>
+      </c>
+      <c r="G2" t="s">
+        <v>380</v>
+      </c>
+      <c r="H2" t="s">
+        <v>381</v>
+      </c>
+      <c r="I2" t="s">
+        <v>383</v>
+      </c>
+      <c r="J2" t="s">
+        <v>385</v>
+      </c>
+      <c r="K2" t="s">
+        <v>387</v>
+      </c>
+      <c r="L2" t="s">
+        <v>389</v>
+      </c>
+      <c r="M2" t="s">
+        <v>391</v>
+      </c>
+      <c r="N2" t="s">
         <v>396</v>
       </c>
-      <c r="B2" t="s">
-        <v>370</v>
-      </c>
-      <c r="C2" t="s">
-        <v>377</v>
-      </c>
-      <c r="D2" t="s">
-        <v>378</v>
-      </c>
-      <c r="E2" t="s">
-        <v>379</v>
-      </c>
-      <c r="F2" t="s">
-        <v>380</v>
-      </c>
-      <c r="G2" t="s">
-        <v>381</v>
-      </c>
-      <c r="H2" t="s">
-        <v>382</v>
-      </c>
-      <c r="I2" t="s">
-        <v>384</v>
-      </c>
-      <c r="J2" t="s">
-        <v>386</v>
-      </c>
-      <c r="K2" t="s">
-        <v>388</v>
-      </c>
-      <c r="L2" t="s">
-        <v>390</v>
-      </c>
-      <c r="M2" t="s">
-        <v>392</v>
-      </c>
-      <c r="N2" t="s">
-        <v>397</v>
-      </c>
       <c r="O2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="P2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
   </sheetData>
@@ -6461,93 +6481,93 @@
         <v>68</v>
       </c>
       <c r="C1" t="s">
+        <v>370</v>
+      </c>
+      <c r="D1" t="s">
         <v>371</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>372</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>373</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>374</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>375</v>
       </c>
-      <c r="H1" t="s">
-        <v>376</v>
-      </c>
       <c r="I1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="J1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="K1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="L1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="M1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="N1" t="s">
+        <v>392</v>
+      </c>
+      <c r="O1" t="s">
         <v>393</v>
-      </c>
-      <c r="O1" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C2" t="s">
+        <v>376</v>
+      </c>
+      <c r="D2" t="s">
         <v>377</v>
       </c>
-      <c r="D2" t="s">
-        <v>378</v>
-      </c>
       <c r="E2" t="s">
+        <v>397</v>
+      </c>
+      <c r="F2" t="s">
+        <v>379</v>
+      </c>
+      <c r="G2" t="s">
+        <v>380</v>
+      </c>
+      <c r="H2" t="s">
         <v>398</v>
       </c>
-      <c r="F2" t="s">
-        <v>380</v>
-      </c>
-      <c r="G2" t="s">
-        <v>381</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>383</v>
+      </c>
+      <c r="J2" t="s">
+        <v>385</v>
+      </c>
+      <c r="K2" t="s">
         <v>399</v>
       </c>
-      <c r="I2" t="s">
-        <v>384</v>
-      </c>
-      <c r="J2" t="s">
-        <v>386</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
+        <v>389</v>
+      </c>
+      <c r="M2" t="s">
+        <v>391</v>
+      </c>
+      <c r="N2" t="s">
         <v>400</v>
       </c>
-      <c r="L2" t="s">
-        <v>390</v>
-      </c>
-      <c r="M2" t="s">
-        <v>392</v>
-      </c>
-      <c r="N2" t="s">
-        <v>401</v>
-      </c>
       <c r="O2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="P2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
   </sheetData>
@@ -6616,8 +6636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{292FBDAE-D596-4C82-A946-FDA545BEF94C}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6637,55 +6657,55 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>401</v>
+      </c>
+      <c r="B1" t="s">
         <v>402</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>403</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>404</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>405</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>406</v>
       </c>
-      <c r="F1" t="s">
-        <v>407</v>
-      </c>
       <c r="G1" t="s">
+        <v>409</v>
+      </c>
+      <c r="H1" t="s">
         <v>410</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>411</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>412</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>413</v>
       </c>
-      <c r="K1" t="s">
-        <v>414</v>
-      </c>
       <c r="L1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B2" s="7" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>26/07/2025</v>
+        <v>03/08/2025</v>
       </c>
       <c r="C2" t="s">
+        <v>407</v>
+      </c>
+      <c r="D2" t="s">
         <v>408</v>
-      </c>
-      <c r="D2" t="s">
-        <v>409</v>
       </c>
       <c r="E2" t="s">
         <v>302</v>
@@ -6694,19 +6714,19 @@
         <v>117</v>
       </c>
       <c r="H2" t="s">
+        <v>414</v>
+      </c>
+      <c r="I2" t="s">
         <v>415</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>416</v>
       </c>
-      <c r="J2" t="s">
-        <v>417</v>
-      </c>
       <c r="K2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="L2" t="s">
-        <v>421</v>
+        <v>658</v>
       </c>
     </row>
   </sheetData>
@@ -6874,16 +6894,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>426</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>427</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>428</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>429</v>
       </c>
     </row>
   </sheetData>
@@ -6896,7 +6916,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6920,66 +6940,66 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>428</v>
+      </c>
+      <c r="B1" t="s">
+        <v>429</v>
+      </c>
+      <c r="C1" t="s">
         <v>430</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>431</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>432</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>433</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>434</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>435</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>436</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>437</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>438</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>439</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>440</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>441</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>442</v>
-      </c>
-      <c r="N1" t="s">
-        <v>443</v>
-      </c>
-      <c r="O1" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>443</v>
+      </c>
+      <c r="B2" t="s">
+        <v>444</v>
+      </c>
+      <c r="C2" t="s">
         <v>445</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>446</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" s="6" t="s">
         <v>447</v>
-      </c>
-      <c r="D2" t="s">
-        <v>448</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>449</v>
       </c>
       <c r="F2" t="str">
         <f>LOWER(G2)</f>
@@ -6993,7 +7013,7 @@
         <v>internal</v>
       </c>
       <c r="I2" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="J2" t="str">
         <f>LOWER(K2)</f>
@@ -7003,17 +7023,17 @@
         <v>103</v>
       </c>
       <c r="L2" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="M2" t="str">
         <f>LOWER(N2)</f>
         <v>implanted</v>
       </c>
       <c r="N2" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
   </sheetData>
@@ -7051,86 +7071,86 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>428</v>
+      </c>
+      <c r="B1" t="s">
+        <v>429</v>
+      </c>
+      <c r="C1" t="s">
         <v>430</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>431</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>452</v>
+      </c>
+      <c r="F1" t="s">
         <v>432</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>433</v>
       </c>
-      <c r="E1" t="s">
-        <v>454</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>434</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>435</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>436</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>437</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>438</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>439</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>440</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>441</v>
       </c>
-      <c r="N1" t="s">
-        <v>442</v>
-      </c>
-      <c r="O1" t="s">
-        <v>443</v>
-      </c>
       <c r="P1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>443</v>
+      </c>
+      <c r="B2" t="s">
+        <v>454</v>
+      </c>
+      <c r="C2" t="s">
         <v>445</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>455</v>
+      </c>
+      <c r="E2" t="s">
         <v>456</v>
       </c>
-      <c r="C2" t="s">
-        <v>447</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="F2" s="6" t="s">
         <v>457</v>
-      </c>
-      <c r="E2" t="s">
-        <v>458</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>459</v>
       </c>
       <c r="G2" t="str">
         <f>SUBSTITUTE(LOWER(H2)," ","")</f>
         <v>firststage</v>
       </c>
       <c r="H2" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="I2" t="str">
         <f>LOWER(J2)</f>
         <v>external</v>
       </c>
       <c r="J2" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="K2" t="str">
         <f>LOWER(L2)</f>
@@ -7140,7 +7160,7 @@
         <v>184</v>
       </c>
       <c r="M2" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="N2" t="str">
         <f>LOWER(O2)</f>
@@ -7150,7 +7170,7 @@
         <v>204</v>
       </c>
       <c r="P2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
   </sheetData>
@@ -7183,126 +7203,126 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>462</v>
+      </c>
+      <c r="B1" t="s">
+        <v>463</v>
+      </c>
+      <c r="C1" t="s">
         <v>464</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>465</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>466</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>467</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>468</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>469</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>470</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>471</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>472</v>
-      </c>
-      <c r="J1" t="s">
-        <v>473</v>
-      </c>
-      <c r="K1" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>473</v>
+      </c>
+      <c r="B2" t="s">
+        <v>474</v>
+      </c>
+      <c r="C2" t="s">
         <v>475</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>476</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>477</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>478</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>479</v>
       </c>
-      <c r="F2" t="s">
+      <c r="K2" t="s">
         <v>480</v>
-      </c>
-      <c r="G2" t="s">
-        <v>481</v>
-      </c>
-      <c r="K2" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>481</v>
+      </c>
+      <c r="B3" t="s">
+        <v>482</v>
+      </c>
+      <c r="C3" t="s">
         <v>483</v>
-      </c>
-      <c r="B3" t="s">
-        <v>484</v>
-      </c>
-      <c r="C3" t="s">
-        <v>485</v>
       </c>
       <c r="D3" t="s">
         <v>100</v>
       </c>
       <c r="K3" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>485</v>
+      </c>
+      <c r="B4" t="s">
+        <v>486</v>
+      </c>
+      <c r="C4" t="s">
         <v>487</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>488</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>489</v>
       </c>
-      <c r="D4" t="s">
+      <c r="K4" t="s">
         <v>490</v>
-      </c>
-      <c r="E4" t="s">
-        <v>491</v>
-      </c>
-      <c r="K4" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>491</v>
+      </c>
+      <c r="B5" t="s">
+        <v>492</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>493</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>494</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="E5" t="s">
         <v>495</v>
       </c>
-      <c r="D5" t="s">
-        <v>496</v>
-      </c>
-      <c r="E5" t="s">
-        <v>497</v>
-      </c>
       <c r="F5" t="s">
+        <v>492</v>
+      </c>
+      <c r="G5" t="s">
+        <v>493</v>
+      </c>
+      <c r="H5" t="s">
         <v>494</v>
-      </c>
-      <c r="G5" t="s">
-        <v>495</v>
-      </c>
-      <c r="H5" t="s">
-        <v>496</v>
       </c>
       <c r="I5" t="s">
         <v>100</v>
@@ -7311,7 +7331,7 @@
         <v>100</v>
       </c>
       <c r="K5" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -7351,43 +7371,43 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>462</v>
+      </c>
+      <c r="B1" t="s">
+        <v>463</v>
+      </c>
+      <c r="C1" t="s">
         <v>464</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>465</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>466</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>467</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>468</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>469</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>470</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>471</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>472</v>
       </c>
-      <c r="J1" t="s">
-        <v>473</v>
-      </c>
-      <c r="K1" t="s">
-        <v>474</v>
-      </c>
       <c r="L1" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="M1" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="N1" t="s">
         <v>122</v>
@@ -7395,118 +7415,118 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B2" t="s">
+        <v>499</v>
+      </c>
+      <c r="C2" t="s">
+        <v>500</v>
+      </c>
+      <c r="D2" t="s">
         <v>501</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>502</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>503</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>504</v>
       </c>
-      <c r="F2" t="s">
+      <c r="K2" t="s">
         <v>505</v>
       </c>
-      <c r="G2" t="s">
+      <c r="L2" s="5" t="s">
         <v>506</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" s="5" t="s">
+        <v>506</v>
+      </c>
+      <c r="N2" t="s">
         <v>507</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>508</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>508</v>
-      </c>
-      <c r="N2" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B3" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="C3" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D3" t="s">
         <v>60</v>
       </c>
       <c r="K3" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="N3" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B4" t="s">
+        <v>511</v>
+      </c>
+      <c r="C4" t="s">
+        <v>512</v>
+      </c>
+      <c r="D4" t="s">
         <v>513</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>514</v>
       </c>
-      <c r="D4" t="s">
+      <c r="K4" t="s">
         <v>515</v>
       </c>
-      <c r="E4" t="s">
-        <v>516</v>
-      </c>
-      <c r="K4" t="s">
-        <v>517</v>
-      </c>
       <c r="L4" s="5" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="N4" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>491</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>493</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" t="s">
+        <v>494</v>
+      </c>
+      <c r="D5" t="s">
         <v>495</v>
       </c>
-      <c r="C5" t="s">
-        <v>496</v>
-      </c>
-      <c r="D5" t="s">
-        <v>497</v>
-      </c>
       <c r="E5" t="s">
+        <v>492</v>
+      </c>
+      <c r="F5" t="s">
+        <v>493</v>
+      </c>
+      <c r="G5" t="s">
         <v>494</v>
       </c>
-      <c r="F5" t="s">
-        <v>495</v>
-      </c>
-      <c r="G5" t="s">
-        <v>496</v>
-      </c>
       <c r="H5" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="I5" t="s">
         <v>60</v>
@@ -7515,16 +7535,16 @@
         <v>60</v>
       </c>
       <c r="K5" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="N5" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
   </sheetData>
@@ -7567,160 +7587,160 @@
         <v>68</v>
       </c>
       <c r="B1" t="s">
+        <v>517</v>
+      </c>
+      <c r="C1" t="s">
+        <v>518</v>
+      </c>
+      <c r="D1" t="s">
         <v>519</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>520</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>521</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>522</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>523</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>524</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>525</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>526</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>527</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>528</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>529</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>530</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>531</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>532</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>533</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>534</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>535</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>536</v>
-      </c>
-      <c r="T1" t="s">
-        <v>537</v>
-      </c>
-      <c r="U1" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>537</v>
+      </c>
+      <c r="B2" t="s">
+        <v>538</v>
+      </c>
+      <c r="C2" t="s">
         <v>539</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>540</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>541</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>542</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>543</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>544</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>545</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>546</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>547</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>548</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>549</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>550</v>
       </c>
-      <c r="M2" t="s">
+      <c r="P2" t="s">
         <v>551</v>
       </c>
-      <c r="N2" t="s">
+      <c r="Q2" t="s">
         <v>552</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>553</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>554</v>
       </c>
-      <c r="R2" t="s">
-        <v>555</v>
-      </c>
-      <c r="S2" t="s">
-        <v>556</v>
-      </c>
       <c r="U2" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>555</v>
+      </c>
+      <c r="B3" t="s">
+        <v>556</v>
+      </c>
+      <c r="C3" t="s">
         <v>557</v>
-      </c>
-      <c r="B3" t="s">
-        <v>558</v>
-      </c>
-      <c r="C3" t="s">
-        <v>559</v>
       </c>
       <c r="D3" t="s">
         <v>314</v>
       </c>
       <c r="O3" t="s">
+        <v>558</v>
+      </c>
+      <c r="T3" t="s">
+        <v>559</v>
+      </c>
+      <c r="U3" t="s">
         <v>560</v>
-      </c>
-      <c r="T3" t="s">
-        <v>561</v>
-      </c>
-      <c r="U3" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>561</v>
+      </c>
+      <c r="O4" t="s">
+        <v>562</v>
+      </c>
+      <c r="T4" t="s">
         <v>563</v>
       </c>
-      <c r="O4" t="s">
+      <c r="U4" t="s">
         <v>564</v>
-      </c>
-      <c r="T4" t="s">
-        <v>565</v>
-      </c>
-      <c r="U4" t="s">
-        <v>566</v>
       </c>
     </row>
   </sheetData>
@@ -7766,70 +7786,70 @@
         <v>68</v>
       </c>
       <c r="B1" t="s">
+        <v>517</v>
+      </c>
+      <c r="C1" t="s">
+        <v>518</v>
+      </c>
+      <c r="D1" t="s">
         <v>519</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>520</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>521</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>522</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>523</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>524</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>525</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>526</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>527</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>528</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>529</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>530</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>531</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>532</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>533</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>534</v>
       </c>
-      <c r="R1" t="s">
-        <v>535</v>
-      </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>536</v>
-      </c>
-      <c r="T1" t="s">
-        <v>538</v>
       </c>
       <c r="U1" t="s">
         <v>132</v>
       </c>
       <c r="V1" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="W1" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="X1" t="s">
         <v>122</v>
@@ -7837,93 +7857,93 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>537</v>
+      </c>
+      <c r="B2" t="s">
+        <v>542</v>
+      </c>
+      <c r="C2" t="s">
+        <v>543</v>
+      </c>
+      <c r="D2" t="s">
+        <v>567</v>
+      </c>
+      <c r="E2" t="s">
+        <v>568</v>
+      </c>
+      <c r="F2" t="s">
+        <v>538</v>
+      </c>
+      <c r="G2" t="s">
         <v>539</v>
       </c>
-      <c r="B2" t="s">
-        <v>544</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="H2" t="s">
+        <v>569</v>
+      </c>
+      <c r="I2" t="s">
+        <v>548</v>
+      </c>
+      <c r="J2" t="s">
+        <v>549</v>
+      </c>
+      <c r="K2" t="s">
+        <v>570</v>
+      </c>
+      <c r="L2" t="s">
         <v>545</v>
       </c>
-      <c r="D2" t="s">
-        <v>569</v>
-      </c>
-      <c r="E2" t="s">
-        <v>570</v>
-      </c>
-      <c r="F2" t="s">
-        <v>540</v>
-      </c>
-      <c r="G2" t="s">
-        <v>541</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="M2" t="s">
+        <v>546</v>
+      </c>
+      <c r="N2" t="s">
         <v>571</v>
       </c>
-      <c r="I2" t="s">
-        <v>550</v>
-      </c>
-      <c r="J2" t="s">
-        <v>551</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="P2" t="s">
         <v>572</v>
       </c>
-      <c r="L2" t="s">
-        <v>547</v>
-      </c>
-      <c r="M2" t="s">
-        <v>548</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="Q2" t="s">
         <v>573</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>574</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>575</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
+        <v>537</v>
+      </c>
+      <c r="U2" s="5" t="s">
         <v>576</v>
       </c>
-      <c r="S2" t="s">
+      <c r="V2" s="5" t="s">
+        <v>576</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>576</v>
+      </c>
+      <c r="X2" t="s">
         <v>577</v>
-      </c>
-      <c r="T2" t="s">
-        <v>539</v>
-      </c>
-      <c r="U2" s="5" t="s">
-        <v>578</v>
-      </c>
-      <c r="V2" s="5" t="s">
-        <v>578</v>
-      </c>
-      <c r="W2" s="5" t="s">
-        <v>578</v>
-      </c>
-      <c r="X2" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>578</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>579</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>580</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>581</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>582</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>186</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -7934,45 +7954,45 @@
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
       <c r="O3" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="T3" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="V3" s="5" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="W3" s="5" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="X3" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>583</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>584</v>
+      </c>
+      <c r="O4" t="s">
         <v>585</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="T4" t="s">
+        <v>564</v>
+      </c>
+      <c r="V4" s="5" t="s">
         <v>586</v>
       </c>
-      <c r="O4" t="s">
-        <v>587</v>
-      </c>
-      <c r="T4" t="s">
-        <v>566</v>
-      </c>
-      <c r="V4" s="5" t="s">
-        <v>588</v>
-      </c>
       <c r="W4" s="5" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="X4" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -8014,108 +8034,108 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>587</v>
+      </c>
+      <c r="B1" t="s">
+        <v>588</v>
+      </c>
+      <c r="C1" t="s">
         <v>589</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>590</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>591</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>592</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>593</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>594</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>595</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>596</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>597</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>598</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>599</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>600</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>601</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>602</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>603</v>
-      </c>
-      <c r="P1" t="s">
-        <v>604</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="B2" t="s">
+        <v>605</v>
+      </c>
+      <c r="C2" t="s">
+        <v>606</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>607</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" s="6" t="s">
         <v>608</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="F2" t="s">
         <v>609</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="G2" t="s">
         <v>610</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>611</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>612</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>613</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>614</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>615</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>616</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>617</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>618</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>619</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" s="10" t="s">
         <v>620</v>
-      </c>
-      <c r="P2" t="s">
-        <v>621</v>
-      </c>
-      <c r="Q2" s="10" t="s">
-        <v>622</v>
       </c>
     </row>
   </sheetData>
@@ -8171,121 +8191,121 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>587</v>
+      </c>
+      <c r="B1" t="s">
+        <v>588</v>
+      </c>
+      <c r="C1" t="s">
+        <v>621</v>
+      </c>
+      <c r="D1" t="s">
         <v>589</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>590</v>
       </c>
-      <c r="C1" t="s">
-        <v>623</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>591</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>622</v>
+      </c>
+      <c r="H1" t="s">
         <v>592</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>593</v>
       </c>
-      <c r="G1" t="s">
-        <v>624</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>594</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>595</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>596</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>597</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>598</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>599</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>600</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>601</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>602</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>603</v>
-      </c>
-      <c r="R1" t="s">
-        <v>604</v>
-      </c>
-      <c r="S1" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="B2" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="C2" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="D2" t="str">
         <f>LOWER(C2)</f>
         <v>withdrawn</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>607</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="H2" t="s">
         <v>609</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>423</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>423</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>610</v>
+      </c>
+      <c r="J2" t="s">
         <v>611</v>
       </c>
-      <c r="I2" t="s">
-        <v>612</v>
-      </c>
-      <c r="J2" t="s">
-        <v>613</v>
-      </c>
       <c r="K2" t="s">
+        <v>624</v>
+      </c>
+      <c r="L2" t="s">
+        <v>625</v>
+      </c>
+      <c r="M2" t="s">
         <v>626</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>627</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>628</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>629</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>630</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>631</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" s="10" t="s">
         <v>632</v>
-      </c>
-      <c r="R2" t="s">
-        <v>633</v>
-      </c>
-      <c r="S2" s="10" t="s">
-        <v>634</v>
       </c>
     </row>
   </sheetData>
@@ -8350,7 +8370,7 @@
         <v>214</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="D2" t="s">
         <v>125</v>
@@ -8420,7 +8440,7 @@
         <v>198</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="C2" t="s">
         <v>125</v>
@@ -8441,6 +8461,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="563c2453-77f6-4899-a3ec-7eb6553b4f66">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="c9416fa7-6169-4354-a691-3cfdebf72cd6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100957D2DE5FA4F58469907EC3226CC7D98" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="090753d51dfd09a1119d54c5de179dfc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="563c2453-77f6-4899-a3ec-7eb6553b4f66" xmlns:ns3="c9416fa7-6169-4354-a691-3cfdebf72cd6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9c8570d9b0f0a7b9a0c34f8b658bbfee" ns2:_="" ns3:_="">
     <xsd:import namespace="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
@@ -8695,27 +8735,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="563c2453-77f6-4899-a3ec-7eb6553b4f66">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="c9416fa7-6169-4354-a691-3cfdebf72cd6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE0B556D-2173-4F7C-9F53-AE9A9D15CB9C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
+    <ds:schemaRef ds:uri="c9416fa7-6169-4354-a691-3cfdebf72cd6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{101DBEFA-2EFF-47B2-92EB-3E72B43EE2A6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1EC2FBF-A56D-40AC-8C09-CB1DCD191DD4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8732,23 +8771,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE0B556D-2173-4F7C-9F53-AE9A9D15CB9C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
-    <ds:schemaRef ds:uri="c9416fa7-6169-4354-a691-3cfdebf72cd6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{101DBEFA-2EFF-47B2-92EB-3E72B43EE2A6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Push allergy Save button change
</commit_message>
<xml_diff>
--- a/ExcelFiles/PatientSummary.xlsx
+++ b/ExcelFiles/PatientSummary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riomed\Release_Server\Cellma4ClinicalAuto2\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F528392F-88CA-4773-B6AC-47BFD4CD3DEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EFBD600-5D5C-42DC-99D6-746C538BCE9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="24" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="64" activeTab="70" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginDetails" sheetId="2" r:id="rId1"/>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1339" uniqueCount="694">
   <si>
     <t>username</t>
   </si>
@@ -2092,9 +2092,6 @@
     <t>Value</t>
   </si>
   <si>
-    <t>Blood Pressure (35)</t>
-  </si>
-  <si>
     <t>Blood Pressure Diastolic (mmHg)</t>
   </si>
   <si>
@@ -2177,6 +2174,21 @@
   </si>
   <si>
     <t>Weight (kg) (kg)</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>125</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>Respiratory Rate (Breaths per Minute) (bpm)</t>
   </si>
 </sst>
 </file>
@@ -2186,7 +2198,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\/mm\/yyyy"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2213,6 +2225,12 @@
       <color rgb="FFAF00DB"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0C0B0B"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2242,7 +2260,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2274,6 +2292,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3729,7 +3748,7 @@
       </c>
       <c r="D2" s="6" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>07/09/2025</v>
+        <v>14/09/2025</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>196</v>
@@ -3808,7 +3827,7 @@
       </c>
       <c r="D2" s="6" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>07/09/2025</v>
+        <v>14/09/2025</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>197</v>
@@ -3874,7 +3893,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9AC72BC-1449-4578-8E57-945920649F3D}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -4054,7 +4073,7 @@
       </c>
       <c r="C2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45907</v>
+        <v>45914</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>103</v>
@@ -6793,7 +6812,7 @@
       </c>
       <c r="B2" s="7" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>07/09/2025</v>
+        <v>14/09/2025</v>
       </c>
       <c r="C2" t="s">
         <v>407</v>
@@ -8411,8 +8430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1409E8F-5957-4174-90DF-2D056EF65E2C}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8430,56 +8449,56 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>661</v>
-      </c>
-      <c r="B2">
-        <v>120</v>
+      <c r="A2" s="17" t="s">
+        <v>693</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>689</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>662</v>
-      </c>
-      <c r="B3">
-        <v>75</v>
+        <v>661</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>578</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>663</v>
-      </c>
-      <c r="B4">
-        <v>80</v>
+        <v>662</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>690</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>664</v>
-      </c>
-      <c r="B5">
-        <v>125</v>
+        <v>663</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>691</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>665</v>
-      </c>
-      <c r="B6">
-        <v>99</v>
+        <v>664</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>692</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>666</v>
-      </c>
-      <c r="B7">
-        <v>99</v>
+        <v>665</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>692</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -8487,7 +8506,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B9">
         <v>72</v>
@@ -8495,7 +8514,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B10">
         <v>68</v>
@@ -8503,7 +8522,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B11">
         <v>52</v>
@@ -8511,7 +8530,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B12">
         <v>162</v>
@@ -8519,7 +8538,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B13">
         <v>168</v>
@@ -8527,7 +8546,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B14">
         <v>61</v>
@@ -8535,7 +8554,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B15">
         <v>100</v>
@@ -8543,7 +8562,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B16">
         <v>18</v>
@@ -8551,7 +8570,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B17">
         <v>102</v>
@@ -8559,7 +8578,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B18">
         <v>98</v>
@@ -8567,7 +8586,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B19">
         <v>99</v>
@@ -8575,7 +8594,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B20">
         <v>55</v>
@@ -8583,7 +8602,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B21">
         <v>69</v>
@@ -8591,7 +8610,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B22">
         <v>298</v>
@@ -8599,7 +8618,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B23">
         <v>78</v>
@@ -8607,7 +8626,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B24">
         <v>48</v>
@@ -8615,7 +8634,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B25">
         <v>298</v>
@@ -8623,7 +8642,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B26">
         <v>19</v>
@@ -8631,7 +8650,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B27">
         <v>65</v>
@@ -8639,7 +8658,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B28">
         <v>89</v>
@@ -8647,7 +8666,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B29">
         <v>36</v>
@@ -8655,7 +8674,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B30">
         <v>58</v>
@@ -8663,6 +8682,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8814,6 +8834,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="563c2453-77f6-4899-a3ec-7eb6553b4f66">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="c9416fa7-6169-4354-a691-3cfdebf72cd6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100957D2DE5FA4F58469907EC3226CC7D98" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="090753d51dfd09a1119d54c5de179dfc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="563c2453-77f6-4899-a3ec-7eb6553b4f66" xmlns:ns3="c9416fa7-6169-4354-a691-3cfdebf72cd6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9c8570d9b0f0a7b9a0c34f8b658bbfee" ns2:_="" ns3:_="">
     <xsd:import namespace="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
@@ -9068,27 +9108,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="563c2453-77f6-4899-a3ec-7eb6553b4f66">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="c9416fa7-6169-4354-a691-3cfdebf72cd6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE0B556D-2173-4F7C-9F53-AE9A9D15CB9C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
+    <ds:schemaRef ds:uri="c9416fa7-6169-4354-a691-3cfdebf72cd6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{101DBEFA-2EFF-47B2-92EB-3E72B43EE2A6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1EC2FBF-A56D-40AC-8C09-CB1DCD191DD4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9105,23 +9144,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE0B556D-2173-4F7C-9F53-AE9A9D15CB9C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
-    <ds:schemaRef ds:uri="c9416fa7-6169-4354-a691-3cfdebf72cd6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{101DBEFA-2EFF-47B2-92EB-3E72B43EE2A6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Push code for medication remove notes
</commit_message>
<xml_diff>
--- a/ExcelFiles/PatientSummary.xlsx
+++ b/ExcelFiles/PatientSummary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riomed\Release_Server\Cellma4ClinicalAuto2\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26282DF4-E4F5-4242-B889-27D141B01249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63989498-38BF-4628-BDF6-1CE090AA3A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="57" activeTab="62" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="60" activeTab="62" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginDetails" sheetId="2" r:id="rId1"/>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1336" uniqueCount="691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1336" uniqueCount="692">
   <si>
     <t>username</t>
   </si>
@@ -2180,6 +2180,9 @@
   </si>
   <si>
     <t>Cochlear Implantation (7/31/2025, left)</t>
+  </si>
+  <si>
+    <t>Cochlear Implantation (01/08/2025, Left)</t>
   </si>
 </sst>
 </file>
@@ -3739,7 +3742,7 @@
       </c>
       <c r="D2" s="6" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>18/10/2025</v>
+        <v>01/11/2025</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>196</v>
@@ -3818,7 +3821,7 @@
       </c>
       <c r="D2" s="6" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>18/10/2025</v>
+        <v>01/11/2025</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>197</v>
@@ -4064,7 +4067,7 @@
       </c>
       <c r="C2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45948</v>
+        <v>45962</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>103</v>
@@ -5448,7 +5451,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5535,7 +5538,7 @@
         <v>306</v>
       </c>
       <c r="H2" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="I2" t="s">
         <v>100</v>
@@ -6803,7 +6806,7 @@
       </c>
       <c r="B2" s="7" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>18/10/2025</v>
+        <v>01/11/2025</v>
       </c>
       <c r="C2" t="s">
         <v>407</v>
@@ -7020,7 +7023,7 @@
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7097,7 +7100,7 @@
         <v>444</v>
       </c>
       <c r="C2" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="D2" t="s">
         <v>446</v>
@@ -8723,26 +8726,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="563c2453-77f6-4899-a3ec-7eb6553b4f66">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="c9416fa7-6169-4354-a691-3cfdebf72cd6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100957D2DE5FA4F58469907EC3226CC7D98" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="090753d51dfd09a1119d54c5de179dfc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="563c2453-77f6-4899-a3ec-7eb6553b4f66" xmlns:ns3="c9416fa7-6169-4354-a691-3cfdebf72cd6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9c8570d9b0f0a7b9a0c34f8b658bbfee" ns2:_="" ns3:_="">
     <xsd:import namespace="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
@@ -8997,26 +8980,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE0B556D-2173-4F7C-9F53-AE9A9D15CB9C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
-    <ds:schemaRef ds:uri="c9416fa7-6169-4354-a691-3cfdebf72cd6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="563c2453-77f6-4899-a3ec-7eb6553b4f66">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="c9416fa7-6169-4354-a691-3cfdebf72cd6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{101DBEFA-2EFF-47B2-92EB-3E72B43EE2A6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1EC2FBF-A56D-40AC-8C09-CB1DCD191DD4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9033,4 +9017,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE0B556D-2173-4F7C-9F53-AE9A9D15CB9C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
+    <ds:schemaRef ds:uri="c9416fa7-6169-4354-a691-3cfdebf72cd6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{101DBEFA-2EFF-47B2-92EB-3E72B43EE2A6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Condition change to Past medical history
</commit_message>
<xml_diff>
--- a/ExcelFiles/PatientSummary.xlsx
+++ b/ExcelFiles/PatientSummary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riomed\Release_Server\Cellma4ClinicalAuto2\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2862615-6BC1-4098-8EED-5B866D9D0E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A19C68-4535-42B4-86C5-95DEBD4F272D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="42" activeTab="47" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="45" activeTab="50" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginDetails" sheetId="2" r:id="rId1"/>
@@ -2068,9 +2068,6 @@
     <t>Rash</t>
   </si>
   <si>
-    <t>Conditions</t>
-  </si>
-  <si>
     <t>Asthmatic bronchitis</t>
   </si>
   <si>
@@ -2189,6 +2186,9 @@
   </si>
   <si>
     <t>Urgent</t>
+  </si>
+  <si>
+    <t>Past Medical History</t>
   </si>
 </sst>
 </file>
@@ -3748,7 +3748,7 @@
       </c>
       <c r="D2" s="6" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>12/11/2025</v>
+        <v>22/11/2025</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>196</v>
@@ -3827,7 +3827,7 @@
       </c>
       <c r="D2" s="6" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>12/11/2025</v>
+        <v>22/11/2025</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>197</v>
@@ -4073,7 +4073,7 @@
       </c>
       <c r="C2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45973</v>
+        <v>45983</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>103</v>
@@ -5529,7 +5529,7 @@
         <v>282</v>
       </c>
       <c r="B2" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>204</v>
@@ -5562,7 +5562,7 @@
         <v>303</v>
       </c>
       <c r="N2" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="O2" t="s">
         <v>301</v>
@@ -5583,7 +5583,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{132C5A93-3712-47E8-A929-16017ECD465E}">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
@@ -5670,7 +5670,7 @@
         <v>282</v>
       </c>
       <c r="B2" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>308</v>
@@ -5703,7 +5703,7 @@
         <v>303</v>
       </c>
       <c r="N2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="O2" t="s">
         <v>301</v>
@@ -5737,7 +5737,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5771,16 +5771,16 @@
     </row>
     <row r="2" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>693</v>
+      </c>
+      <c r="B2" t="s">
         <v>653</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="6" t="s">
         <v>654</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>655</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>656</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>322</v>
@@ -5976,7 +5976,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6010,10 +6010,10 @@
     </row>
     <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>693</v>
+      </c>
+      <c r="B2" t="s">
         <v>653</v>
-      </c>
-      <c r="B2" t="s">
-        <v>654</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>320</v>
@@ -6037,8 +6037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06A0A6C0-CF2F-48B8-BAC5-F3E5690001A5}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6060,10 +6060,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>693</v>
+      </c>
+      <c r="B2" t="s">
         <v>653</v>
-      </c>
-      <c r="B2" t="s">
-        <v>654</v>
       </c>
       <c r="C2" t="s">
         <v>123</v>
@@ -6812,7 +6812,7 @@
       </c>
       <c r="B2" s="7" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>12/11/2025</v>
+        <v>22/11/2025</v>
       </c>
       <c r="C2" t="s">
         <v>407</v>
@@ -6839,7 +6839,7 @@
         <v>418</v>
       </c>
       <c r="L2" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
   </sheetData>
@@ -7106,7 +7106,7 @@
         <v>444</v>
       </c>
       <c r="C2" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D2" t="s">
         <v>446</v>
@@ -7151,7 +7151,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -8452,111 +8452,111 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>657</v>
+      </c>
+      <c r="B1" t="s">
         <v>658</v>
-      </c>
-      <c r="B1" t="s">
-        <v>659</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>314</v>
@@ -8564,18 +8564,18 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
   </sheetData>
@@ -8732,17 +8732,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="563c2453-77f6-4899-a3ec-7eb6553b4f66">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="c9416fa7-6169-4354-a691-3cfdebf72cd6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -8751,7 +8740,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100957D2DE5FA4F58469907EC3226CC7D98" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="090753d51dfd09a1119d54c5de179dfc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="563c2453-77f6-4899-a3ec-7eb6553b4f66" xmlns:ns3="c9416fa7-6169-4354-a691-3cfdebf72cd6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9c8570d9b0f0a7b9a0c34f8b658bbfee" ns2:_="" ns3:_="">
     <xsd:import namespace="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
@@ -9006,18 +8995,18 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE0B556D-2173-4F7C-9F53-AE9A9D15CB9C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
-    <ds:schemaRef ds:uri="c9416fa7-6169-4354-a691-3cfdebf72cd6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="563c2453-77f6-4899-a3ec-7eb6553b4f66">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="c9416fa7-6169-4354-a691-3cfdebf72cd6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{101DBEFA-2EFF-47B2-92EB-3E72B43EE2A6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -9025,7 +9014,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1EC2FBF-A56D-40AC-8C09-CB1DCD191DD4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9042,4 +9031,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE0B556D-2173-4F7C-9F53-AE9A9D15CB9C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
+    <ds:schemaRef ds:uri="c9416fa7-6169-4354-a691-3cfdebf72cd6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Push physical sign excel
</commit_message>
<xml_diff>
--- a/ExcelFiles/PatientSummary.xlsx
+++ b/ExcelFiles/PatientSummary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riomed\Release_Server\Cellma4ClinicalAuto2\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D50C7E-62B9-4637-993C-059C83A4B5EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC62B18E-5BBA-4FE2-A461-44209B011B9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="64" activeTab="70" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginDetails" sheetId="2" r:id="rId1"/>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1336" uniqueCount="694">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1334" uniqueCount="692">
   <si>
     <t>username</t>
   </si>
@@ -2113,9 +2113,6 @@
     <t>Height (cm)</t>
   </si>
   <si>
-    <t>Height(cm) (cm)</t>
-  </si>
-  <si>
     <t>O/E - respiratory rate (bpm)</t>
   </si>
   <si>
@@ -2138,9 +2135,6 @@
   </si>
   <si>
     <t>160</t>
-  </si>
-  <si>
-    <t>162</t>
   </si>
   <si>
     <t>100</t>
@@ -2630,7 +2624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5682E5CD-63B5-4779-9930-5C9E9312DCA8}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2650,7 +2644,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="B2" t="s">
         <v>123</v>
@@ -3748,7 +3742,7 @@
       </c>
       <c r="D2" s="6" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>22/11/2025</v>
+        <v>23/11/2025</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>196</v>
@@ -3827,7 +3821,7 @@
       </c>
       <c r="D2" s="6" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>22/11/2025</v>
+        <v>23/11/2025</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>197</v>
@@ -4073,7 +4067,7 @@
       </c>
       <c r="C2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45983</v>
+        <v>45984</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>103</v>
@@ -5529,7 +5523,7 @@
         <v>281</v>
       </c>
       <c r="B2" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>203</v>
@@ -5562,7 +5556,7 @@
         <v>302</v>
       </c>
       <c r="N2" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="O2" t="s">
         <v>300</v>
@@ -5670,7 +5664,7 @@
         <v>281</v>
       </c>
       <c r="B2" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>307</v>
@@ -5703,7 +5697,7 @@
         <v>302</v>
       </c>
       <c r="N2" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="O2" t="s">
         <v>300</v>
@@ -5771,7 +5765,7 @@
     </row>
     <row r="2" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="B2" t="s">
         <v>652</v>
@@ -6010,7 +6004,7 @@
     </row>
     <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="B2" t="s">
         <v>652</v>
@@ -6060,7 +6054,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="B2" t="s">
         <v>652</v>
@@ -6812,7 +6806,7 @@
       </c>
       <c r="B2" s="7" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>22/11/2025</v>
+        <v>23/11/2025</v>
       </c>
       <c r="C2" t="s">
         <v>406</v>
@@ -7106,7 +7100,7 @@
         <v>443</v>
       </c>
       <c r="C2" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="D2" t="s">
         <v>445</v>
@@ -7151,7 +7145,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -8438,10 +8432,10 @@
 
 <file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1409E8F-5957-4174-90DF-2D056EF65E2C}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8471,7 +8465,7 @@
         <v>665</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -8487,7 +8481,7 @@
         <v>667</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -8495,55 +8489,55 @@
         <v>668</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>669</v>
+        <v>658</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>658</v>
+        <v>669</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>670</v>
+        <v>659</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>661</v>
+        <v>670</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -8551,7 +8545,7 @@
         <v>671</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>684</v>
+        <v>313</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -8559,7 +8553,7 @@
         <v>672</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>313</v>
+        <v>683</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -8567,15 +8561,7 @@
         <v>673</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>674</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
   </sheetData>
@@ -8635,7 +8621,7 @@
     </row>
     <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="B2" t="s">
         <v>213</v>
@@ -8708,7 +8694,7 @@
     </row>
     <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>646</v>
@@ -8732,15 +8718,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100957D2DE5FA4F58469907EC3226CC7D98" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="090753d51dfd09a1119d54c5de179dfc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="563c2453-77f6-4899-a3ec-7eb6553b4f66" xmlns:ns3="c9416fa7-6169-4354-a691-3cfdebf72cd6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9c8570d9b0f0a7b9a0c34f8b658bbfee" ns2:_="" ns3:_="">
     <xsd:import namespace="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
@@ -8995,7 +8972,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="563c2453-77f6-4899-a3ec-7eb6553b4f66">
@@ -9006,15 +8983,16 @@
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{101DBEFA-2EFF-47B2-92EB-3E72B43EE2A6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1EC2FBF-A56D-40AC-8C09-CB1DCD191DD4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9033,7 +9011,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE0B556D-2173-4F7C-9F53-AE9A9D15CB9C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9042,4 +9020,12 @@
     <ds:schemaRef ds:uri="c9416fa7-6169-4354-a691-3cfdebf72cd6"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{101DBEFA-2EFF-47B2-92EB-3E72B43EE2A6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>